<commit_message>
better resulst, ults and tiered tables
</commit_message>
<xml_diff>
--- a/mean_results/avg_ensemble_results_80_20_optimize_F1.xlsx
+++ b/mean_results/avg_ensemble_results_80_20_optimize_F1.xlsx
@@ -498,474 +498,474 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>AdaBoostClassifier_LogisticRegression</t>
+          <t>BaggingClassifier_RandomForestClassifier</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7425787545787544</v>
+        <v>0.7418051948051948</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5337469198149296</v>
+        <v>0.7786215084275305</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4838082953176926</v>
+        <v>0.6381502664002663</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7698268928134289</v>
+        <v>0.7514722867664044</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4934006657188313</v>
+        <v>0.7452074243364226</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4475405603971312</v>
+        <v>0.626876507936508</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6333333333333333</v>
+        <v>0.6523200584581659</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6139098786417971</v>
+        <v>0.8353756063996794</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5663624126988356</v>
+        <v>0.69384</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0.9243421052631579</v>
       </c>
       <c r="L2" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>0.09464907149858126</v>
+        <v>0.0708401703481492</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>BaggingClassifier_LGBMClassifier</t>
+          <t>AdaBoostClassifier_ElasticNet</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7136689976689976</v>
+        <v>0.7365094905094904</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8733647911354719</v>
+        <v>0.6063306186985057</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5809030225330225</v>
+        <v>0.5902592607392607</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7651593988436094</v>
+        <v>0.7302255639097744</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8661901780916154</v>
+        <v>0.5145723803342735</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5899834126984127</v>
+        <v>0.5061193650793649</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6611904761904761</v>
+        <v>0.625</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8902265474613195</v>
+        <v>0.7734045189663428</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6046533333333334</v>
+        <v>0.7562800000000001</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9414473684210526</v>
+        <v>0.9263157894736842</v>
       </c>
       <c r="L3" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M3" t="n">
-        <v>0.09092928809225945</v>
+        <v>0.07432284238523497</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>BaggingClassifier_RandomForestClassifier</t>
+          <t>BaggingClassifier_MLPClassifier</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.737011655011655</v>
+        <v>0.7468154068154067</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8527909190758578</v>
+        <v>0.7778592126706385</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6252037296037296</v>
+        <v>0.5848579498279498</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7361528401850983</v>
+        <v>0.7221852708694814</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8248864370600254</v>
+        <v>0.74969256562834</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6109026984126984</v>
+        <v>0.561708253968254</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6727743271221532</v>
+        <v>0.6346432552954292</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8920984930098609</v>
+        <v>0.8495767761114266</v>
       </c>
       <c r="J4" t="n">
-        <v>0.6724333333333332</v>
+        <v>0.65908</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8745813397129186</v>
+        <v>0.9052631578947368</v>
       </c>
       <c r="L4" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M4" t="n">
-        <v>0.09697885328142003</v>
+        <v>0.09239425066899742</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>BaggingClassifier_SVC</t>
+          <t>BaggingClassifier_ElasticNet</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7386666666666666</v>
+        <v>0.7216464646464646</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6653087283582019</v>
+        <v>0.7111949035344317</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5402471850371851</v>
+        <v>0.6145594560994561</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7342591773551526</v>
+        <v>0.7192539261504779</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6246185056852193</v>
+        <v>0.6953775892605648</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5027438095238095</v>
+        <v>0.6204036507936508</v>
       </c>
       <c r="H5" t="n">
-        <v>0.635</v>
+        <v>0.6627075098814229</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7643579987455975</v>
+        <v>0.7561323883006558</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6418333333333333</v>
+        <v>0.6574933333333333</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9263157894736842</v>
+        <v>0.8822368421052632</v>
       </c>
       <c r="L5" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M5" t="n">
-        <v>0.07180795124394949</v>
+        <v>0.08715056708979337</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>AdaBoostClassifier_ElasticNet</t>
+          <t>AdaBoostClassifier_LogisticRegression</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7365094905094904</v>
+        <v>0.7065534465534465</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6063306186985057</v>
+        <v>0.4486190254095954</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5902592607392607</v>
+        <v>0.3939958103039225</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7302255639097744</v>
+        <v>0.7161350143628354</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5145723803342735</v>
+        <v>0.455165632397839</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5061193650793649</v>
+        <v>0.4052426473737031</v>
       </c>
       <c r="H6" t="n">
-        <v>0.625</v>
+        <v>0.691437908496732</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7734045189663428</v>
+        <v>0.4638884506696695</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7562800000000001</v>
+        <v>0.4165537311068794</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9263157894736842</v>
+        <v>0.8083732057416269</v>
       </c>
       <c r="L6" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M6" t="n">
-        <v>0.07432284238523497</v>
+        <v>0.0838032356257451</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>BaggingClassifier_LogisticRegression</t>
+          <t>AdaBoostClassifier_RandomForestClassifier</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.744187923187923</v>
+        <v>0.688030525030525</v>
       </c>
       <c r="C7" t="n">
-        <v>0.647592956349476</v>
+        <v>0.9745644978593611</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5363543483531867</v>
+        <v>0.5826053046953047</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7264160401002506</v>
+        <v>0.6916026625704046</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6249804192829418</v>
+        <v>0.9729430391231592</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5234931691795182</v>
+        <v>0.5839711111111111</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6321428571428571</v>
+        <v>0.6861904761904762</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7008586732619956</v>
+        <v>0.9769140836738405</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5912970313580732</v>
+        <v>0.6056666666666667</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9157894736842106</v>
+        <v>0.7481203007518797</v>
       </c>
       <c r="L7" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M7" t="n">
-        <v>0.07759100588143095</v>
+        <v>0.03375418510784727</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>BaggingClassifier_MLPClassifier</t>
+          <t>BaggingClassifier_SVC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7468154068154067</v>
+        <v>0.5752582972582972</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7778592126706385</v>
+        <v>0.6786090912849334</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5848579498279498</v>
+        <v>0.5032424797424797</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7221852708694814</v>
+        <v>0.6884686688913607</v>
       </c>
       <c r="F8" t="n">
-        <v>0.74969256562834</v>
+        <v>0.8117157808385528</v>
       </c>
       <c r="G8" t="n">
-        <v>0.561708253968254</v>
+        <v>0.6207037037037038</v>
       </c>
       <c r="H8" t="n">
-        <v>0.6346432552954292</v>
+        <v>0.7135689903491762</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8495767761114266</v>
+        <v>0.605933864908029</v>
       </c>
       <c r="J8" t="n">
-        <v>0.65908</v>
+        <v>0.4673888888888889</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9052631578947368</v>
+        <v>0.702828092959672</v>
       </c>
       <c r="L8" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M8" t="n">
-        <v>0.09239425066899742</v>
+        <v>0.06903845900034065</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>BaggingClassifier_ElasticNet</t>
+          <t>BaggingClassifier_LogisticRegression</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7216464646464646</v>
+        <v>0.6722009102009101</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7111949035344317</v>
+        <v>0.3772383746203655</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6145594560994561</v>
+        <v>0.3742643005143005</v>
       </c>
       <c r="E9" t="n">
-        <v>0.7192539261504779</v>
+        <v>0.6870729492573812</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6953775892605648</v>
+        <v>0.3253572391019477</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6204036507936508</v>
+        <v>0.3226597222222222</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6627075098814229</v>
+        <v>0.7374206349206349</v>
       </c>
       <c r="I9" t="n">
-        <v>0.7561323883006558</v>
+        <v>0.4810153619458331</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6574933333333333</v>
+        <v>0.4813888888888889</v>
       </c>
       <c r="K9" t="n">
-        <v>0.8822368421052632</v>
+        <v>0.6630297334244702</v>
       </c>
       <c r="L9" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M9" t="n">
-        <v>0.08715056708979337</v>
+        <v>0.07602264282925202</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>BaggingClassifier_DecisionTreeClassifier</t>
+          <t>BaggingClassifier_LGBMClassifier</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6958532578532578</v>
+        <v>0.6731740481740481</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8291357656341306</v>
+        <v>0.8734972280535755</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5684385534465535</v>
+        <v>0.5512636874236874</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7110317460317461</v>
+        <v>0.6583206237855194</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8490092371392153</v>
+        <v>0.8953046919062156</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5958104444444444</v>
+        <v>0.5940509523809524</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6530325814536341</v>
+        <v>0.6643496372908138</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8206983366623245</v>
+        <v>0.8576943050870103</v>
       </c>
       <c r="J10" t="n">
-        <v>0.5734586666666667</v>
+        <v>0.5434733333333334</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8208219412166781</v>
+        <v>0.6717703349282297</v>
       </c>
       <c r="L10" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0629493171376205</v>
+        <v>0.107010038859451</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>AdaBoostClassifier_RandomForestClassifier</t>
+          <t>AdaBoostClassifier_LGBMClassifier</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.688030525030525</v>
+        <v>0.6523377733377733</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9745644978593611</v>
+        <v>0.9636394380414736</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5826053046953047</v>
+        <v>0.5320437917637918</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6916026625704046</v>
+        <v>0.6337049127343246</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9729430391231592</v>
+        <v>0.9743356864131657</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5839711111111111</v>
+        <v>0.5696755555555555</v>
       </c>
       <c r="H11" t="n">
-        <v>0.6861904761904762</v>
+        <v>0.6364147548358075</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9769140836738405</v>
+        <v>0.9541319255077918</v>
       </c>
       <c r="J11" t="n">
-        <v>0.6056666666666667</v>
+        <v>0.52408</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7481203007518797</v>
+        <v>0.6470095693779905</v>
       </c>
       <c r="L11" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M11" t="n">
-        <v>0.03375418510784727</v>
+        <v>0.1102829514060827</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>AdaBoostClassifier_LGBMClassifier</t>
+          <t>BaggingClassifier_DecisionTreeClassifier</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.6661652791652791</v>
+        <v>0.641087912087912</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9591233654016804</v>
+        <v>0.8193019912900767</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5532150427350427</v>
+        <v>0.5612277278277278</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6633228840125392</v>
+        <v>0.6300389776251846</v>
       </c>
       <c r="F12" t="n">
-        <v>0.958847192399863</v>
+        <v>0.8533034117617351</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5727774603174604</v>
+        <v>0.6117920634920635</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6705968541262659</v>
+        <v>0.587703449800973</v>
       </c>
       <c r="I12" t="n">
-        <v>0.961245729872964</v>
+        <v>0.7987459252331593</v>
       </c>
       <c r="J12" t="n">
-        <v>0.5601333333333333</v>
+        <v>0.5501333333333334</v>
       </c>
       <c r="K12" t="n">
-        <v>0.6812115516062884</v>
+        <v>0.6831937799043062</v>
       </c>
       <c r="L12" t="n">
         <v>64.40000000000001</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0873078115221109</v>
+        <v>0.1381285326917519</v>
       </c>
     </row>
     <row r="13">

</xml_diff>